<commit_message>
Fixed bugs in soi processing.
</commit_message>
<xml_diff>
--- a/Data/Calibration/Firm Calibration/data/soi/data/soi_partner/Crosswalks/12pa01_Crosswalk.xlsx
+++ b/Data/Calibration/Firm Calibration/data/soi/data/soi_partner/Crosswalks/12pa01_Crosswalk.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Lott, Sherwin\Firm Calibration\data\soi\data\soi_partner\Crosswalks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sherwin.lott\Documents\Firm Calibration\data\soi\data\soi_partner\Crosswalks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -431,9 +431,6 @@
     <t>Industry:</t>
   </si>
   <si>
-    <t>NAICS Code:</t>
-  </si>
-  <si>
     <t>8112.8113.8114</t>
   </si>
   <si>
@@ -444,6 +441,9 @@
   </si>
   <si>
     <t>Other real estate activities</t>
+  </si>
+  <si>
+    <t>Codes:</t>
   </si>
 </sst>
 </file>
@@ -781,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +795,7 @@
         <v>134</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B96" s="4"/>
     </row>
@@ -1625,7 +1625,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -1646,7 +1646,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B108" s="4">
         <v>5419</v>
@@ -1857,7 +1857,7 @@
         <v>130</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>